<commit_message>
Load nutrition dataset from CSV, auto populate CVX array, fix unit conversions, display full constraint results, and support multiple user scenarios. - MH
</commit_message>
<xml_diff>
--- a/Datasets/food_data_with_prices.xlsx
+++ b/Datasets/food_data_with_prices.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentuncc-my.sharepoint.com/personal/mhasan21_charlotte_edu/Documents/2025_Fall/ECGR_5115 - Convex Opt/Project/Diet_Nutrition/Datasets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_FFC65FC0B2412FE1DC170BFE0BC15B5D49119B53" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B779315-ED50-480D-BA68-12CCF7590290}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="2530" yWindow="780" windowWidth="28350" windowHeight="19950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -301,8 +307,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -365,13 +371,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -409,7 +423,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -443,6 +457,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -477,9 +492,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -652,14 +668,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:38">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -775,7 +799,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:38">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -816,7 +840,7 @@
         <v>14.6</v>
       </c>
       <c r="N2">
-        <v>0.016</v>
+        <v>1.6E-2</v>
       </c>
       <c r="O2">
         <v>7.6</v>
@@ -825,28 +849,28 @@
         <v>0.2</v>
       </c>
       <c r="Q2">
-        <v>0.033</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="R2">
-        <v>0.064</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="S2">
-        <v>0.092</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="T2">
-        <v>0.097</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="U2">
-        <v>0.08400000000000001</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="V2">
-        <v>0.052</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="W2">
-        <v>0.096</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="X2">
-        <v>0.004</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="Y2">
         <v>0</v>
@@ -858,40 +882,40 @@
         <v>0.1</v>
       </c>
       <c r="AB2">
-        <v>0.008</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="AC2">
         <v>14.1</v>
       </c>
       <c r="AD2">
-        <v>0.082</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="AE2">
-        <v>0.027</v>
+        <v>2.7E-2</v>
       </c>
       <c r="AF2">
         <v>1.3</v>
       </c>
       <c r="AG2">
-        <v>0.091</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="AH2">
         <v>15.5</v>
       </c>
       <c r="AI2">
-        <v>19.1</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="AJ2">
-        <v>0.039</v>
+        <v>3.9E-2</v>
       </c>
       <c r="AK2">
         <v>7.07</v>
       </c>
       <c r="AL2">
-        <v>0.004</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:38">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>10</v>
       </c>
@@ -914,13 +938,13 @@
         <v>0.4</v>
       </c>
       <c r="H3">
-        <v>0.036</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="I3">
         <v>0.7</v>
       </c>
       <c r="J3">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="K3">
         <v>1.4</v>
@@ -932,64 +956,64 @@
         <v>4.3</v>
       </c>
       <c r="N3">
-        <v>0.043</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="O3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="P3">
-        <v>0.017</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="Q3">
-        <v>0.003</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="R3">
-        <v>0.015</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="S3">
-        <v>0.091</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="T3">
-        <v>0.081</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="U3">
-        <v>0.077</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="V3">
-        <v>0.057</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="W3">
-        <v>0.077</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="X3">
-        <v>0.007</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="Y3">
         <v>0</v>
       </c>
       <c r="Z3">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AA3">
-        <v>0.014</v>
+        <v>1.4E-2</v>
       </c>
       <c r="AB3">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="AC3">
         <v>42.7</v>
       </c>
       <c r="AD3">
-        <v>0.094</v>
+        <v>9.4E-2</v>
       </c>
       <c r="AE3">
-        <v>0.094</v>
+        <v>9.4E-2</v>
       </c>
       <c r="AF3">
         <v>1.7</v>
       </c>
       <c r="AG3">
-        <v>0.026</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="AH3">
         <v>31.4</v>
@@ -998,16 +1022,16 @@
         <v>9</v>
       </c>
       <c r="AJ3">
-        <v>0.038</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="AK3">
-        <v>3.745</v>
+        <v>3.7450000000000001</v>
       </c>
       <c r="AL3">
-        <v>0.0145</v>
+        <v>1.4500000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:38">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>20</v>
       </c>
@@ -1054,46 +1078,46 @@
         <v>12.3</v>
       </c>
       <c r="P4">
-        <v>0.016</v>
+        <v>1.6E-2</v>
       </c>
       <c r="Q4">
-        <v>0.042</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="R4">
-        <v>0.059</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="S4">
-        <v>0.074</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="T4">
         <v>0.1</v>
       </c>
       <c r="U4">
-        <v>0.08500000000000001</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="V4">
-        <v>0.08599999999999999</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="W4">
-        <v>0.033</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="X4">
         <v>0</v>
       </c>
       <c r="Y4">
-        <v>0.042</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="Z4">
-        <v>0.07199999999999999</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="AA4">
-        <v>0.064</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="AB4">
         <v>202.2</v>
       </c>
       <c r="AC4">
-        <v>0.093</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="AD4">
         <v>0.1</v>
@@ -1102,28 +1126,28 @@
         <v>7.2</v>
       </c>
       <c r="AF4">
-        <v>0.08500000000000001</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="AG4">
-        <v>135.3</v>
+        <v>135.30000000000001</v>
       </c>
       <c r="AH4">
-        <v>40.8</v>
+        <v>40.799999999999997</v>
       </c>
       <c r="AI4">
-        <v>0.056</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="AJ4">
         <v>0.8</v>
       </c>
       <c r="AK4">
-        <v>219.002</v>
+        <v>219.00200000000001</v>
       </c>
       <c r="AL4">
-        <v>0.0045</v>
+        <v>4.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:38">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>30</v>
       </c>
@@ -1137,7 +1161,7 @@
         <v>98</v>
       </c>
       <c r="E5">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="F5">
         <v>5</v>
@@ -1173,52 +1197,52 @@
         <v>0.1</v>
       </c>
       <c r="Q5">
-        <v>0.021</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="R5">
-        <v>0.095</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="S5">
-        <v>0.082</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="T5">
         <v>0.2</v>
       </c>
       <c r="U5">
-        <v>0.008999999999999999</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="V5">
         <v>0.4</v>
       </c>
       <c r="W5">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="X5">
         <v>0</v>
       </c>
       <c r="Y5">
-        <v>0.004</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="Z5">
-        <v>0.055</v>
+        <v>5.5E-2</v>
       </c>
       <c r="AA5">
-        <v>0.046</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="AB5">
         <v>149.1</v>
       </c>
       <c r="AC5">
-        <v>0.036</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="AD5">
-        <v>0.011</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="AE5">
         <v>6.3</v>
       </c>
       <c r="AF5">
-        <v>0.054</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="AG5">
         <v>117.9</v>
@@ -1227,19 +1251,19 @@
         <v>38.4</v>
       </c>
       <c r="AI5">
-        <v>0.029</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="AJ5">
         <v>0.6</v>
       </c>
       <c r="AK5">
-        <v>163.575</v>
+        <v>163.57499999999999</v>
       </c>
       <c r="AL5">
-        <v>0.0065</v>
+        <v>6.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:38">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>40</v>
       </c>
@@ -1274,13 +1298,13 @@
         <v>0.08</v>
       </c>
       <c r="L6">
-        <v>0.025</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="M6">
         <v>0</v>
       </c>
       <c r="N6">
-        <v>0.011</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="O6">
         <v>3.6</v>
@@ -1292,22 +1316,22 @@
         <v>0</v>
       </c>
       <c r="R6">
-        <v>0.022</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="S6">
         <v>0</v>
       </c>
       <c r="T6">
-        <v>0.003</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="U6">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="V6">
         <v>0.03</v>
       </c>
       <c r="W6">
-        <v>0.004</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="X6">
         <v>0.1</v>
@@ -1325,16 +1349,16 @@
         <v>1.3</v>
       </c>
       <c r="AC6">
-        <v>0.061</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="AD6">
-        <v>0.017</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="AE6">
         <v>0.4</v>
       </c>
       <c r="AF6">
-        <v>0.098</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="AG6">
         <v>0.8</v>
@@ -1343,19 +1367,19 @@
         <v>10.9</v>
       </c>
       <c r="AI6">
-        <v>0.021</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AJ6">
-        <v>0.008</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="AK6">
-        <v>18.892</v>
+        <v>18.891999999999999</v>
       </c>
       <c r="AL6">
-        <v>0.008</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:38">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>50</v>
       </c>
@@ -1378,7 +1402,7 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.062</v>
+        <v>6.2E-2</v>
       </c>
       <c r="I7">
         <v>1.4</v>
@@ -1393,7 +1417,7 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>8.800000000000001</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="N7">
         <v>0.3</v>
@@ -1402,76 +1426,76 @@
         <v>7.6</v>
       </c>
       <c r="P7">
-        <v>0.043</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="Q7">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="R7">
-        <v>0.066</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="S7">
-        <v>0.022</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="T7">
-        <v>0.076</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="U7">
-        <v>0.089</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="V7">
         <v>0.1</v>
       </c>
       <c r="W7">
-        <v>0.08599999999999999</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="X7">
         <v>0</v>
       </c>
       <c r="Y7">
-        <v>0.014</v>
+        <v>1.4E-2</v>
       </c>
       <c r="Z7">
-        <v>0.022</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="AA7">
-        <v>0.046</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="AB7">
-        <v>89.90000000000001</v>
+        <v>89.9</v>
       </c>
       <c r="AC7">
-        <v>0.061</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="AD7">
-        <v>0.079</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="AE7">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AF7">
-        <v>0.062</v>
+        <v>6.2E-2</v>
       </c>
       <c r="AG7">
         <v>140</v>
       </c>
       <c r="AH7">
-        <v>38.7</v>
+        <v>38.700000000000003</v>
       </c>
       <c r="AI7">
-        <v>0.052</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="AJ7">
         <v>0.4</v>
       </c>
       <c r="AK7">
-        <v>97.357</v>
+        <v>97.356999999999999</v>
       </c>
       <c r="AL7">
-        <v>0.0042</v>
+        <v>4.1999999999999997E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:38">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>60</v>
       </c>
@@ -1485,7 +1509,7 @@
         <v>323</v>
       </c>
       <c r="E8">
-        <v>17.6</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="F8">
         <v>9</v>
@@ -1509,7 +1533,7 @@
         <v>0</v>
       </c>
       <c r="M8">
-        <v>40.3</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="N8">
         <v>1.3</v>
@@ -1518,16 +1542,16 @@
         <v>128.4</v>
       </c>
       <c r="P8">
-        <v>0.016</v>
+        <v>1.6E-2</v>
       </c>
       <c r="Q8">
-        <v>0.056</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="R8">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="S8">
-        <v>0.036</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="T8">
         <v>0.4</v>
@@ -1563,7 +1587,7 @@
         <v>3.1</v>
       </c>
       <c r="AE8">
-        <v>82.59999999999999</v>
+        <v>82.6</v>
       </c>
       <c r="AF8">
         <v>0.6</v>
@@ -1575,19 +1599,19 @@
         <v>574.1</v>
       </c>
       <c r="AI8">
-        <v>0.092</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="AJ8">
         <v>2.7</v>
       </c>
       <c r="AK8">
-        <v>292.933</v>
+        <v>292.93299999999999</v>
       </c>
       <c r="AL8">
-        <v>0.0055</v>
+        <v>5.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:38">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>70</v>
       </c>
@@ -1601,7 +1625,7 @@
         <v>350</v>
       </c>
       <c r="E9">
-        <v>17.6</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="F9">
         <v>3.3</v>
@@ -1613,7 +1637,7 @@
         <v>8.4</v>
       </c>
       <c r="I9">
-        <v>33.2</v>
+        <v>33.200000000000003</v>
       </c>
       <c r="J9">
         <v>3.9</v>
@@ -1700,10 +1724,10 @@
         <v>114.1</v>
       </c>
       <c r="AL9">
-        <v>0.006</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:38">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>80</v>
       </c>
@@ -1738,7 +1762,7 @@
         <v>5.2</v>
       </c>
       <c r="L10">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -1759,7 +1783,7 @@
         <v>0.04</v>
       </c>
       <c r="S10">
-        <v>0.014</v>
+        <v>1.4E-2</v>
       </c>
       <c r="T10">
         <v>0.1</v>
@@ -1783,13 +1807,13 @@
         <v>0.4</v>
       </c>
       <c r="AA10">
-        <v>0.099</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="AB10">
         <v>35.9</v>
       </c>
       <c r="AC10">
-        <v>0.082</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="AD10">
         <v>1.5</v>
@@ -1807,19 +1831,19 @@
         <v>195</v>
       </c>
       <c r="AI10">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="AJ10">
         <v>0.4</v>
       </c>
       <c r="AK10">
-        <v>84.09999999999999</v>
+        <v>84.1</v>
       </c>
       <c r="AL10">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:38">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>90</v>
       </c>
@@ -1842,7 +1866,7 @@
         <v>11.2</v>
       </c>
       <c r="H11">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I11">
         <v>28.8</v>
@@ -1863,7 +1887,7 @@
         <v>0.8</v>
       </c>
       <c r="O11">
-        <v>80.59999999999999</v>
+        <v>80.599999999999994</v>
       </c>
       <c r="P11">
         <v>0.1</v>
@@ -1872,10 +1896,10 @@
         <v>0.6</v>
       </c>
       <c r="R11">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="S11">
-        <v>0.093</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="T11">
         <v>0.4</v>
@@ -1893,13 +1917,13 @@
         <v>0</v>
       </c>
       <c r="Y11">
-        <v>0.063</v>
+        <v>6.3E-2</v>
       </c>
       <c r="Z11">
         <v>1.6</v>
       </c>
       <c r="AA11">
-        <v>0.051</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="AB11">
         <v>277.2</v>
@@ -1923,7 +1947,7 @@
         <v>242.6</v>
       </c>
       <c r="AI11">
-        <v>0.064</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="AJ11">
         <v>1.7</v>
@@ -1932,10 +1956,10 @@
         <v>362.7</v>
       </c>
       <c r="AL11">
-        <v>0.0065</v>
+        <v>6.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:38">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>100</v>
       </c>
@@ -1982,7 +2006,7 @@
         <v>144.6</v>
       </c>
       <c r="P12">
-        <v>0.096</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="Q12">
         <v>0.4</v>
@@ -1991,7 +2015,7 @@
         <v>0.2</v>
       </c>
       <c r="S12">
-        <v>0.08799999999999999</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="T12">
         <v>0.3</v>
@@ -2006,16 +2030,16 @@
         <v>0.5</v>
       </c>
       <c r="X12">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="Y12">
-        <v>0.059</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="Z12">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AA12">
-        <v>0.022</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="AB12">
         <v>216.9</v>
@@ -2024,7 +2048,7 @@
         <v>0.3</v>
       </c>
       <c r="AD12">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AE12">
         <v>60.3</v>
@@ -2036,22 +2060,22 @@
         <v>392.8</v>
       </c>
       <c r="AH12">
-        <v>648.3</v>
+        <v>648.29999999999995</v>
       </c>
       <c r="AI12">
-        <v>0.031</v>
+        <v>3.1E-2</v>
       </c>
       <c r="AJ12">
         <v>4.8</v>
       </c>
       <c r="AK12">
-        <v>326.183</v>
+        <v>326.18299999999999</v>
       </c>
       <c r="AL12">
-        <v>0.0055</v>
+        <v>5.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:38">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>110</v>
       </c>
@@ -2083,7 +2107,7 @@
         <v>0</v>
       </c>
       <c r="K13">
-        <v>9.699999999999999</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -2095,7 +2119,7 @@
         <v>0.5</v>
       </c>
       <c r="O13">
-        <v>131.3</v>
+        <v>131.30000000000001</v>
       </c>
       <c r="P13">
         <v>0</v>
@@ -2104,7 +2128,7 @@
         <v>0.3</v>
       </c>
       <c r="R13">
-        <v>0.053</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="S13">
         <v>0</v>
@@ -2116,7 +2140,7 @@
         <v>2.5</v>
       </c>
       <c r="V13">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="W13">
         <v>0.2</v>
@@ -2155,7 +2179,7 @@
         <v>787.2</v>
       </c>
       <c r="AI13">
-        <v>0.038</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="AJ13">
         <v>1.2</v>
@@ -2164,10 +2188,10 @@
         <v>109.2</v>
       </c>
       <c r="AL13">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:38">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>120</v>
       </c>
@@ -2217,13 +2241,13 @@
         <v>0.1</v>
       </c>
       <c r="Q14">
-        <v>0.099</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="R14">
         <v>0</v>
       </c>
       <c r="S14">
-        <v>0.066</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="T14">
         <v>0.1</v>
@@ -2247,13 +2271,13 @@
         <v>0.5</v>
       </c>
       <c r="AA14">
-        <v>0.073</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="AB14">
         <v>380.3</v>
       </c>
       <c r="AC14">
-        <v>0.081</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="AD14">
         <v>0.7</v>
@@ -2265,25 +2289,25 @@
         <v>0.1</v>
       </c>
       <c r="AG14">
-        <v>317.1</v>
+        <v>317.10000000000002</v>
       </c>
       <c r="AH14">
         <v>140.4</v>
       </c>
       <c r="AI14">
-        <v>0.07000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="AJ14">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="AK14">
         <v>439.9</v>
       </c>
       <c r="AL14">
-        <v>0.0045</v>
+        <v>4.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:38">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>130</v>
       </c>
@@ -2327,19 +2351,19 @@
         <v>0.3</v>
       </c>
       <c r="O15">
-        <v>34.2</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="P15">
-        <v>0.08799999999999999</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="Q15">
         <v>0.3</v>
       </c>
       <c r="R15">
-        <v>0.083</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="S15">
-        <v>0.08400000000000001</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="T15">
         <v>0.2</v>
@@ -2351,10 +2375,10 @@
         <v>0.3</v>
       </c>
       <c r="W15">
-        <v>0.004</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="X15">
-        <v>0.004</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="Y15">
         <v>0</v>
@@ -2369,7 +2393,7 @@
         <v>36.5</v>
       </c>
       <c r="AC15">
-        <v>0.07199999999999999</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="AD15">
         <v>0.9</v>
@@ -2381,25 +2405,25 @@
         <v>0.1</v>
       </c>
       <c r="AG15">
-        <v>72.90000000000001</v>
+        <v>72.900000000000006</v>
       </c>
       <c r="AH15">
-        <v>88.40000000000001</v>
+        <v>88.4</v>
       </c>
       <c r="AI15">
-        <v>0.065</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="AJ15">
         <v>0.3</v>
       </c>
       <c r="AK15">
-        <v>70.093</v>
+        <v>70.093000000000004</v>
       </c>
       <c r="AL15">
-        <v>0.004</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:38">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>140</v>
       </c>
@@ -2446,19 +2470,19 @@
         <v>29.9</v>
       </c>
       <c r="P16">
-        <v>0.044</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="Q16">
         <v>0.09</v>
       </c>
       <c r="R16">
-        <v>0.065</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="S16">
-        <v>0.041</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="T16">
-        <v>0.006</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="U16">
         <v>0.1</v>
@@ -2488,7 +2512,7 @@
         <v>50.4</v>
       </c>
       <c r="AD16">
-        <v>0.029</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="AE16">
         <v>0.6</v>
@@ -2503,19 +2527,19 @@
         <v>158.4</v>
       </c>
       <c r="AI16">
-        <v>289.6</v>
+        <v>289.60000000000002</v>
       </c>
       <c r="AJ16">
-        <v>0.068</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="AK16">
-        <v>51.581</v>
+        <v>51.581000000000003</v>
       </c>
       <c r="AL16">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:38">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>150</v>
       </c>
@@ -2532,10 +2556,10 @@
         <v>0.5</v>
       </c>
       <c r="F17">
-        <v>0.022</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="G17">
-        <v>0.033</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="H17">
         <v>0.2</v>
@@ -2559,16 +2583,16 @@
         <v>0.2</v>
       </c>
       <c r="O17">
-        <v>9.199999999999999</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="P17">
-        <v>0.097</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="Q17">
         <v>0.2</v>
       </c>
       <c r="R17">
-        <v>0.082</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="S17">
         <v>0</v>
@@ -2580,10 +2604,10 @@
         <v>1.7</v>
       </c>
       <c r="V17">
-        <v>0.051</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="W17">
-        <v>0.007</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="X17">
         <v>0</v>
@@ -2601,10 +2625,10 @@
         <v>15</v>
       </c>
       <c r="AC17">
-        <v>0.039</v>
+        <v>3.9E-2</v>
       </c>
       <c r="AD17">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AE17">
         <v>6.4</v>
@@ -2625,13 +2649,13 @@
         <v>0.2</v>
       </c>
       <c r="AK17">
-        <v>38.815</v>
+        <v>38.814999999999998</v>
       </c>
       <c r="AL17">
-        <v>0.003</v>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>160</v>
       </c>
@@ -2669,7 +2693,7 @@
         <v>0</v>
       </c>
       <c r="M18">
-        <v>275.4</v>
+        <v>275.39999999999998</v>
       </c>
       <c r="N18">
         <v>0.2</v>
@@ -2681,10 +2705,10 @@
         <v>0.1</v>
       </c>
       <c r="Q18">
-        <v>0.092</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="R18">
-        <v>0.036</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="S18">
         <v>0.05</v>
@@ -2711,13 +2735,13 @@
         <v>0.7</v>
       </c>
       <c r="AA18">
-        <v>0.081</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="AB18">
         <v>254</v>
       </c>
       <c r="AC18">
-        <v>0.053</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="AD18">
         <v>1.2</v>
@@ -2726,7 +2750,7 @@
         <v>27.5</v>
       </c>
       <c r="AF18">
-        <v>0.021</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AG18">
         <v>293.8</v>
@@ -2744,10 +2768,10 @@
         <v>351.2</v>
       </c>
       <c r="AL18">
-        <v>0.0055</v>
+        <v>5.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:38">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>170</v>
       </c>
@@ -2767,7 +2791,7 @@
         <v>3.9</v>
       </c>
       <c r="G19">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H19">
         <v>0.5</v>
@@ -2794,16 +2818,16 @@
         <v>32.9</v>
       </c>
       <c r="P19">
-        <v>0.079</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="Q19">
         <v>0.3</v>
       </c>
       <c r="R19">
-        <v>0.051</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="S19">
-        <v>0.038</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="T19">
         <v>0.3</v>
@@ -2815,7 +2839,7 @@
         <v>0</v>
       </c>
       <c r="W19">
-        <v>0.015</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="X19">
         <v>0</v>
@@ -2827,13 +2851,13 @@
         <v>0.2</v>
       </c>
       <c r="AA19">
-        <v>0.08699999999999999</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="AB19">
         <v>164.2</v>
       </c>
       <c r="AC19">
-        <v>0.053</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="AD19">
         <v>1.6</v>
@@ -2848,22 +2872,22 @@
         <v>229</v>
       </c>
       <c r="AH19">
-        <v>96.09999999999999</v>
+        <v>96.1</v>
       </c>
       <c r="AI19">
-        <v>0.064</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="AJ19">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AK19">
-        <v>241.181</v>
+        <v>241.18100000000001</v>
       </c>
       <c r="AL19">
-        <v>0.007</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:38">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>180</v>
       </c>
@@ -2898,10 +2922,10 @@
         <v>10.3</v>
       </c>
       <c r="L20">
-        <v>9.800000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="M20">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="N20">
         <v>0.5</v>
@@ -2916,13 +2940,13 @@
         <v>0.1</v>
       </c>
       <c r="R20">
-        <v>0.099</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="S20">
         <v>0</v>
       </c>
       <c r="T20">
-        <v>0.068</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="U20">
         <v>0.8</v>
@@ -2943,10 +2967,10 @@
         <v>1</v>
       </c>
       <c r="AA20">
-        <v>0.035</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="AB20">
-        <v>93.09999999999999</v>
+        <v>93.1</v>
       </c>
       <c r="AC20">
         <v>0.2</v>
@@ -2967,7 +2991,7 @@
         <v>387.1</v>
       </c>
       <c r="AI20">
-        <v>0.021</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AJ20">
         <v>1.3</v>
@@ -2976,10 +3000,10 @@
         <v>154.4</v>
       </c>
       <c r="AL20">
-        <v>0.0035</v>
+        <v>3.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:38">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>190</v>
       </c>
@@ -3008,10 +3032,10 @@
         <v>1.9</v>
       </c>
       <c r="J21">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K21">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -3032,7 +3056,7 @@
         <v>0.1</v>
       </c>
       <c r="R21">
-        <v>0.048</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="S21">
         <v>0</v>
@@ -3044,10 +3068,10 @@
         <v>1.3</v>
       </c>
       <c r="V21">
-        <v>0.051</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="W21">
-        <v>0.039</v>
+        <v>3.9E-2</v>
       </c>
       <c r="X21">
         <v>0.2</v>
@@ -3056,7 +3080,7 @@
         <v>0</v>
       </c>
       <c r="Z21">
-        <v>0.033</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="AA21">
         <v>0</v>
@@ -3065,7 +3089,7 @@
         <v>12.5</v>
       </c>
       <c r="AC21">
-        <v>0.021</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AD21">
         <v>0.2</v>
@@ -3083,19 +3107,19 @@
         <v>57.3</v>
       </c>
       <c r="AI21">
-        <v>0.058</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="AJ21">
-        <v>0.082</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="AK21">
         <v>17.2</v>
       </c>
       <c r="AL21">
-        <v>0.008</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:38">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>200</v>
       </c>
@@ -3133,7 +3157,7 @@
         <v>1.7</v>
       </c>
       <c r="M22">
-        <v>16.9</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="N22">
         <v>1.7</v>
@@ -3142,16 +3166,16 @@
         <v>207</v>
       </c>
       <c r="P22">
-        <v>0.028</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="Q22">
-        <v>0.061</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="R22">
-        <v>0.093</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="S22">
-        <v>0.076</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="T22">
         <v>0.1</v>
@@ -3163,7 +3187,7 @@
         <v>0.3</v>
       </c>
       <c r="W22">
-        <v>0.013</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="X22">
         <v>1.9</v>
@@ -3175,7 +3199,7 @@
         <v>0.6</v>
       </c>
       <c r="AA22">
-        <v>0.036</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="AB22">
         <v>33.9</v>
@@ -3193,25 +3217,25 @@
         <v>0.7</v>
       </c>
       <c r="AG22">
-        <v>79.90000000000001</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="AH22">
-        <v>304.9</v>
+        <v>304.89999999999998</v>
       </c>
       <c r="AI22">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="AJ22">
         <v>0.7</v>
       </c>
       <c r="AK22">
-        <v>68.983</v>
+        <v>68.983000000000004</v>
       </c>
       <c r="AL22">
-        <v>0.003</v>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:38">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>210</v>
       </c>
@@ -3267,10 +3291,10 @@
         <v>0.1</v>
       </c>
       <c r="S23">
-        <v>0.004</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="T23">
-        <v>0.067</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="U23">
         <v>0.2</v>
@@ -3285,7 +3309,7 @@
         <v>0.3</v>
       </c>
       <c r="Y23">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="Z23">
         <v>0</v>
@@ -3294,7 +3318,7 @@
         <v>2.8</v>
       </c>
       <c r="AB23">
-        <v>0.07199999999999999</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="AC23">
         <v>86.8</v>
@@ -3318,16 +3342,16 @@
         <v>1052</v>
       </c>
       <c r="AJ23">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="AK23">
-        <v>77.607</v>
+        <v>77.606999999999999</v>
       </c>
       <c r="AL23">
-        <v>0.0038</v>
+        <v>3.8E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>220</v>
       </c>
@@ -3365,7 +3389,7 @@
         <v>0</v>
       </c>
       <c r="M24">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="N24">
         <v>0.4</v>
@@ -3374,16 +3398,16 @@
         <v>225.9</v>
       </c>
       <c r="P24">
-        <v>0.036</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="Q24">
-        <v>0.008999999999999999</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="R24">
-        <v>0.07199999999999999</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="S24">
-        <v>0.047</v>
+        <v>4.7E-2</v>
       </c>
       <c r="T24">
         <v>0.2</v>
@@ -3395,7 +3419,7 @@
         <v>0.8</v>
       </c>
       <c r="W24">
-        <v>0.08599999999999999</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="X24">
         <v>0.2</v>
@@ -3416,7 +3440,7 @@
         <v>0.1</v>
       </c>
       <c r="AD24">
-        <v>0.019</v>
+        <v>1.9E-2</v>
       </c>
       <c r="AE24">
         <v>16.3</v>
@@ -3431,7 +3455,7 @@
         <v>335.5</v>
       </c>
       <c r="AI24">
-        <v>0.068</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="AJ24">
         <v>0.1</v>
@@ -3440,10 +3464,10 @@
         <v>14.488</v>
       </c>
       <c r="AL24">
-        <v>0.0045</v>
+        <v>4.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:38">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>230</v>
       </c>
@@ -3460,22 +3484,22 @@
         <v>0.2</v>
       </c>
       <c r="F25">
-        <v>0.07000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G25">
-        <v>0.07099999999999999</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="H25">
-        <v>0.032</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="I25">
         <v>28.1</v>
       </c>
       <c r="J25">
-        <v>0.022</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="K25">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="L25">
         <v>0.2</v>
@@ -3496,7 +3520,7 @@
         <v>0</v>
       </c>
       <c r="R25">
-        <v>0.028</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="S25">
         <v>0</v>
@@ -3511,7 +3535,7 @@
         <v>0.2</v>
       </c>
       <c r="W25">
-        <v>0.029</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="X25">
         <v>0</v>
@@ -3520,7 +3544,7 @@
         <v>0</v>
       </c>
       <c r="Z25">
-        <v>0.092</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="AA25">
         <v>0</v>
@@ -3529,7 +3553,7 @@
         <v>7.3</v>
       </c>
       <c r="AC25">
-        <v>0.004</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AD25">
         <v>0.5</v>
@@ -3547,7 +3571,7 @@
         <v>48.8</v>
       </c>
       <c r="AI25">
-        <v>0.008</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="AJ25">
         <v>0.4</v>
@@ -3556,10 +3580,10 @@
         <v>38.5</v>
       </c>
       <c r="AL25">
-        <v>0.0032</v>
+        <v>3.2000000000000002E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:38">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>240</v>
       </c>
@@ -3573,7 +3597,7 @@
         <v>174</v>
       </c>
       <c r="E26">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="F26">
         <v>2.1</v>
@@ -3591,7 +3615,7 @@
         <v>1.8</v>
       </c>
       <c r="K26">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="L26">
         <v>1</v>
@@ -3606,13 +3630,13 @@
         <v>211.8</v>
       </c>
       <c r="P26">
-        <v>0.091</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="Q26">
         <v>0.1</v>
       </c>
       <c r="R26">
-        <v>0.089</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="S26">
         <v>0</v>
@@ -3627,7 +3651,7 @@
         <v>0.3</v>
       </c>
       <c r="W26">
-        <v>0.033</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="X26">
         <v>5.5</v>
@@ -3657,13 +3681,13 @@
         <v>0.8</v>
       </c>
       <c r="AG26">
-        <v>78.09999999999999</v>
+        <v>78.099999999999994</v>
       </c>
       <c r="AH26">
         <v>347.8</v>
       </c>
       <c r="AI26">
-        <v>0.008999999999999999</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="AJ26">
         <v>1.8</v>
@@ -3672,10 +3696,10 @@
         <v>100.43</v>
       </c>
       <c r="AL26">
-        <v>0.0035</v>
+        <v>3.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:38">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>250</v>
       </c>
@@ -3692,7 +3716,7 @@
         <v>4.3</v>
       </c>
       <c r="F27">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G27">
         <v>1.3</v>
@@ -3701,7 +3725,7 @@
         <v>0.7</v>
       </c>
       <c r="I27">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="J27">
         <v>0</v>
@@ -3716,7 +3740,7 @@
         <v>4.3</v>
       </c>
       <c r="N27">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="O27">
         <v>194.7</v>
@@ -3725,25 +3749,25 @@
         <v>0</v>
       </c>
       <c r="Q27">
-        <v>0.019</v>
+        <v>1.9E-2</v>
       </c>
       <c r="R27">
-        <v>0.048</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="S27">
-        <v>0.008999999999999999</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="T27">
-        <v>0.08599999999999999</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="U27">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="V27">
         <v>0.3</v>
       </c>
       <c r="W27">
-        <v>0.017</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="X27">
         <v>0.2</v>
@@ -3770,7 +3794,7 @@
         <v>15.1</v>
       </c>
       <c r="AF27">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AG27">
         <v>45.4</v>
@@ -3788,10 +3812,10 @@
         <v>43.2</v>
       </c>
       <c r="AL27">
-        <v>0.025</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:38">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>260</v>
       </c>
@@ -3808,7 +3832,7 @@
         <v>10.1</v>
       </c>
       <c r="F28">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G28">
         <v>3.4</v>
@@ -3838,16 +3862,16 @@
         <v>29.3</v>
       </c>
       <c r="P28">
-        <v>0.07099999999999999</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="Q28">
-        <v>0.045</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="R28">
         <v>0</v>
       </c>
       <c r="S28">
-        <v>0.028</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="T28">
         <v>0.1</v>
@@ -3895,19 +3919,19 @@
         <v>135.1</v>
       </c>
       <c r="AI28">
-        <v>0.064</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="AJ28">
         <v>1</v>
       </c>
       <c r="AK28">
-        <v>41.248</v>
+        <v>41.247999999999998</v>
       </c>
       <c r="AL28">
-        <v>0.008500000000000001</v>
+        <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:38">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>270</v>
       </c>
@@ -3933,7 +3957,7 @@
         <v>0.5</v>
       </c>
       <c r="I29">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="J29">
         <v>2.1</v>
@@ -3948,7 +3972,7 @@
         <v>0</v>
       </c>
       <c r="N29">
-        <v>0.014</v>
+        <v>1.4E-2</v>
       </c>
       <c r="O29">
         <v>7</v>
@@ -3957,7 +3981,7 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>0.066</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="R29">
         <v>0</v>
@@ -3966,16 +3990,16 @@
         <v>0</v>
       </c>
       <c r="T29">
-        <v>0.039</v>
+        <v>3.9E-2</v>
       </c>
       <c r="U29">
         <v>0.5</v>
       </c>
       <c r="V29">
-        <v>0.07199999999999999</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="W29">
-        <v>0.037</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="X29">
         <v>0</v>
@@ -3987,13 +4011,13 @@
         <v>0.2</v>
       </c>
       <c r="AA29">
-        <v>0.008999999999999999</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="AB29">
         <v>11.1</v>
       </c>
       <c r="AC29">
-        <v>0.036</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="AD29">
         <v>0.4</v>
@@ -4002,7 +4026,7 @@
         <v>4</v>
       </c>
       <c r="AF29">
-        <v>0.068</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="AG29">
         <v>18.3</v>
@@ -4011,7 +4035,7 @@
         <v>23.3</v>
       </c>
       <c r="AI29">
-        <v>0.049</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="AJ29">
         <v>0.1</v>
@@ -4020,10 +4044,10 @@
         <v>25.5</v>
       </c>
       <c r="AL29">
-        <v>0.0065</v>
+        <v>6.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:38">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>280</v>
       </c>
@@ -4049,10 +4073,10 @@
         <v>1.3</v>
       </c>
       <c r="I30">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="J30">
-        <v>0.053</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="K30">
         <v>3.9</v>
@@ -4070,19 +4094,19 @@
         <v>13.9</v>
       </c>
       <c r="P30">
-        <v>0.08799999999999999</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="Q30">
-        <v>0.096</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="R30">
-        <v>0.083</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="S30">
-        <v>0.054</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="T30">
-        <v>0.032</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="U30">
         <v>0.6</v>
@@ -4091,25 +4115,25 @@
         <v>0.1</v>
       </c>
       <c r="W30">
-        <v>0.06900000000000001</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="X30">
         <v>0</v>
       </c>
       <c r="Y30">
-        <v>0.078</v>
+        <v>7.8E-2</v>
       </c>
       <c r="Z30">
         <v>0.3</v>
       </c>
       <c r="AA30">
-        <v>0.074</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="AB30">
         <v>3.9</v>
       </c>
       <c r="AC30">
-        <v>0.027</v>
+        <v>2.7E-2</v>
       </c>
       <c r="AD30">
         <v>0.6</v>
@@ -4118,28 +4142,28 @@
         <v>4.2</v>
       </c>
       <c r="AF30">
-        <v>0.049</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="AG30">
-        <v>75.59999999999999</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="AH30">
         <v>77</v>
       </c>
       <c r="AI30">
-        <v>0.054</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="AJ30">
         <v>0.4</v>
       </c>
       <c r="AK30">
-        <v>17.934</v>
+        <v>17.934000000000001</v>
       </c>
       <c r="AL30">
-        <v>0.007</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:38">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>290</v>
       </c>
@@ -4189,16 +4213,16 @@
         <v>0</v>
       </c>
       <c r="Q31">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="R31">
         <v>0</v>
       </c>
       <c r="S31">
-        <v>0.006</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="T31">
-        <v>0.015</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="U31">
         <v>4</v>
@@ -4219,13 +4243,13 @@
         <v>0.4</v>
       </c>
       <c r="AA31">
-        <v>0.092</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="AB31">
         <v>11.8</v>
       </c>
       <c r="AC31">
-        <v>0.014</v>
+        <v>1.4E-2</v>
       </c>
       <c r="AD31">
         <v>0.3</v>
@@ -4243,7 +4267,7 @@
         <v>156.5</v>
       </c>
       <c r="AI31">
-        <v>0.067</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="AJ31">
         <v>0.3</v>
@@ -4252,10 +4276,10 @@
         <v>35.9</v>
       </c>
       <c r="AL31">
-        <v>0.008999999999999999</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:38">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>300</v>
       </c>
@@ -4308,7 +4332,7 @@
         <v>0.2</v>
       </c>
       <c r="R32">
-        <v>0.011</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="S32">
         <v>0</v>
@@ -4335,10 +4359,10 @@
         <v>2.1</v>
       </c>
       <c r="AA32">
-        <v>0.067</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="AB32">
-        <v>79.90000000000001</v>
+        <v>79.900000000000006</v>
       </c>
       <c r="AC32">
         <v>0.3</v>
@@ -4347,7 +4371,7 @@
         <v>1.8</v>
       </c>
       <c r="AE32">
-        <v>36.3</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="AF32">
         <v>0.4</v>
@@ -4359,7 +4383,7 @@
         <v>561.4</v>
       </c>
       <c r="AI32">
-        <v>0.043</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="AJ32">
         <v>0.9</v>
@@ -4368,10 +4392,10 @@
         <v>127.3</v>
       </c>
       <c r="AL32">
-        <v>0.0055</v>
+        <v>5.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:38">
+    <row r="33" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>310</v>
       </c>
@@ -4400,7 +4424,7 @@
         <v>37.9</v>
       </c>
       <c r="J33">
-        <v>8.800000000000001</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="K33">
         <v>24.1</v>
@@ -4415,7 +4439,7 @@
         <v>0.7</v>
       </c>
       <c r="O33">
-        <v>86.09999999999999</v>
+        <v>86.1</v>
       </c>
       <c r="P33">
         <v>0</v>
@@ -4424,10 +4448,10 @@
         <v>0.3</v>
       </c>
       <c r="R33">
-        <v>0.052</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="S33">
-        <v>0.029</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="T33">
         <v>0.6</v>
@@ -4460,7 +4484,7 @@
         <v>0.2</v>
       </c>
       <c r="AD33">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="AE33">
         <v>37.6</v>
@@ -4478,16 +4502,16 @@
         <v>0</v>
       </c>
       <c r="AJ33">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AK33">
         <v>233.7</v>
       </c>
       <c r="AL33">
-        <v>0.0078</v>
+        <v>7.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:38">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>320</v>
       </c>
@@ -4501,7 +4525,7 @@
         <v>378</v>
       </c>
       <c r="E34">
-        <v>19.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="F34">
         <v>3.8</v>
@@ -4516,7 +4540,7 @@
         <v>35.4</v>
       </c>
       <c r="J34">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="K34">
         <v>15.1</v>
@@ -4540,10 +4564,10 @@
         <v>0.3</v>
       </c>
       <c r="R34">
-        <v>0.073</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="S34">
-        <v>0.054</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="T34">
         <v>0.2</v>
@@ -4567,19 +4591,19 @@
         <v>1.6</v>
       </c>
       <c r="AA34">
-        <v>0.058</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="AB34">
-        <v>160.8</v>
+        <v>160.80000000000001</v>
       </c>
       <c r="AC34">
-        <v>0.025</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AD34">
         <v>2.1</v>
       </c>
       <c r="AE34">
-        <v>36.2</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="AF34">
         <v>0.4</v>
@@ -4591,7 +4615,7 @@
         <v>294.8</v>
       </c>
       <c r="AI34">
-        <v>0.017</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="AJ34">
         <v>0.8</v>
@@ -4600,10 +4624,10 @@
         <v>235.3</v>
       </c>
       <c r="AL34">
-        <v>0.008500000000000001</v>
+        <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:38">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>330</v>
       </c>
@@ -4683,10 +4707,10 @@
         <v>0.3</v>
       </c>
       <c r="AA35">
-        <v>0.008</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="AB35">
-        <v>259.1</v>
+        <v>259.10000000000002</v>
       </c>
       <c r="AC35">
         <v>0.2</v>
@@ -4707,19 +4731,19 @@
         <v>534</v>
       </c>
       <c r="AI35">
-        <v>0.032</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="AJ35">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="AK35">
         <v>405.8</v>
       </c>
       <c r="AL35">
-        <v>0.0075</v>
+        <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:38">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>340</v>
       </c>
@@ -4766,7 +4790,7 @@
         <v>41.6</v>
       </c>
       <c r="P36">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="Q36">
         <v>0.3</v>
@@ -4775,7 +4799,7 @@
         <v>0</v>
       </c>
       <c r="S36">
-        <v>0.033</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="T36">
         <v>0.2</v>
@@ -4799,13 +4823,13 @@
         <v>0.7</v>
       </c>
       <c r="AA36">
-        <v>0.039</v>
+        <v>3.9E-2</v>
       </c>
       <c r="AB36">
         <v>200.6</v>
       </c>
       <c r="AC36">
-        <v>0.003</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="AD36">
         <v>1.9</v>
@@ -4823,19 +4847,19 @@
         <v>166.1</v>
       </c>
       <c r="AI36">
-        <v>0.022</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="AJ36">
         <v>1.6</v>
       </c>
       <c r="AK36">
-        <v>256.272</v>
+        <v>256.27199999999999</v>
       </c>
       <c r="AL36">
-        <v>0.0065</v>
+        <v>6.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:38">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>350</v>
       </c>
@@ -4867,7 +4891,7 @@
         <v>0</v>
       </c>
       <c r="K37">
-        <v>37.7</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="L37">
         <v>0</v>
@@ -4882,7 +4906,7 @@
         <v>100.2</v>
       </c>
       <c r="P37">
-        <v>0.082</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="Q37">
         <v>0.3</v>
@@ -4891,7 +4915,7 @@
         <v>0</v>
       </c>
       <c r="S37">
-        <v>0.027</v>
+        <v>2.7E-2</v>
       </c>
       <c r="T37">
         <v>0.2</v>
@@ -4933,10 +4957,10 @@
         <v>0.1</v>
       </c>
       <c r="AG37">
-        <v>532.8</v>
+        <v>532.79999999999995</v>
       </c>
       <c r="AH37">
-        <v>625.2</v>
+        <v>625.20000000000005</v>
       </c>
       <c r="AI37">
         <v>0.08</v>
@@ -4948,10 +4972,10 @@
         <v>100.864</v>
       </c>
       <c r="AL37">
-        <v>0.018</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:38">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>360</v>
       </c>
@@ -4983,7 +5007,7 @@
         <v>0</v>
       </c>
       <c r="K38">
-        <v>16.9</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="L38">
         <v>0</v>
@@ -4992,22 +5016,22 @@
         <v>60.5</v>
       </c>
       <c r="N38">
-        <v>0.018</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="O38">
         <v>53.8</v>
       </c>
       <c r="P38">
-        <v>0.064</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="Q38">
         <v>0.04</v>
       </c>
       <c r="R38">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="S38">
-        <v>0.045</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="T38">
         <v>0.05</v>
@@ -5025,13 +5049,13 @@
         <v>0</v>
       </c>
       <c r="Y38">
-        <v>0.027</v>
+        <v>2.7E-2</v>
       </c>
       <c r="Z38">
         <v>0.3</v>
       </c>
       <c r="AA38">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="AB38">
         <v>44.6</v>
@@ -5043,10 +5067,10 @@
         <v>0.3</v>
       </c>
       <c r="AE38">
-        <v>19.4</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="AF38">
-        <v>0.017</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="AG38">
         <v>205.2</v>
@@ -5055,19 +5079,19 @@
         <v>312.5</v>
       </c>
       <c r="AI38">
-        <v>0.077</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="AJ38">
         <v>0.4</v>
       </c>
       <c r="AK38">
-        <v>63.037</v>
+        <v>63.036999999999999</v>
       </c>
       <c r="AL38">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:38">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>370</v>
       </c>
@@ -5114,13 +5138,13 @@
         <v>39.4</v>
       </c>
       <c r="P39">
-        <v>0.024</v>
+        <v>2.4E-2</v>
       </c>
       <c r="Q39">
-        <v>0.082</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="R39">
-        <v>0.033</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="S39">
         <v>0</v>
@@ -5135,7 +5159,7 @@
         <v>0</v>
       </c>
       <c r="W39">
-        <v>0.054</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="X39">
         <v>0</v>
@@ -5147,7 +5171,7 @@
         <v>0.05</v>
       </c>
       <c r="AA39">
-        <v>0.059</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="AB39">
         <v>1.2</v>
@@ -5171,19 +5195,19 @@
         <v>1.7</v>
       </c>
       <c r="AI39">
-        <v>0.014</v>
+        <v>1.4E-2</v>
       </c>
       <c r="AJ39">
         <v>0.2</v>
       </c>
       <c r="AK39">
-        <v>6.517</v>
+        <v>6.5170000000000003</v>
       </c>
       <c r="AL39">
         <v>0.02</v>
       </c>
     </row>
-    <row r="40" spans="1:38">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>380</v>
       </c>
@@ -5215,13 +5239,13 @@
         <v>0</v>
       </c>
       <c r="K40">
-        <v>9.800000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="L40">
         <v>0</v>
       </c>
       <c r="M40">
-        <v>33.3</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="N40">
         <v>0.2</v>
@@ -5230,16 +5254,16 @@
         <v>50.4</v>
       </c>
       <c r="P40">
-        <v>0.08699999999999999</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="Q40">
-        <v>0.064</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="R40">
-        <v>0.074</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="S40">
-        <v>0.021</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="T40">
         <v>0.06</v>
@@ -5251,7 +5275,7 @@
         <v>0.2</v>
       </c>
       <c r="W40">
-        <v>0.078</v>
+        <v>7.8E-2</v>
       </c>
       <c r="X40">
         <v>0</v>
@@ -5263,13 +5287,13 @@
         <v>0.5</v>
       </c>
       <c r="AA40">
-        <v>0.051</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="AB40">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="AC40">
-        <v>0.043</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="AD40">
         <v>0.1</v>
@@ -5278,28 +5302,28 @@
         <v>14.7</v>
       </c>
       <c r="AF40">
-        <v>0.045</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="AG40">
-        <v>158.7</v>
+        <v>158.69999999999999</v>
       </c>
       <c r="AH40">
         <v>119.7</v>
       </c>
       <c r="AI40">
-        <v>0.029</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="AJ40">
         <v>0.2</v>
       </c>
       <c r="AK40">
-        <v>28.835</v>
+        <v>28.835000000000001</v>
       </c>
       <c r="AL40">
-        <v>0.0095</v>
+        <v>9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:38">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>390</v>
       </c>
@@ -5340,22 +5364,22 @@
         <v>66</v>
       </c>
       <c r="N41">
-        <v>0.064</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="O41">
         <v>46.9</v>
       </c>
       <c r="P41">
-        <v>0.065</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="Q41">
         <v>0.1</v>
       </c>
       <c r="R41">
-        <v>0.014</v>
+        <v>1.4E-2</v>
       </c>
       <c r="S41">
-        <v>0.097</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="T41">
         <v>0.4</v>
@@ -5385,16 +5409,16 @@
         <v>13.2</v>
       </c>
       <c r="AC41">
-        <v>0.08599999999999999</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="AD41">
         <v>1.4</v>
       </c>
       <c r="AE41">
-        <v>85.40000000000001</v>
+        <v>85.4</v>
       </c>
       <c r="AF41">
-        <v>0.008</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="AG41">
         <v>244.6</v>
@@ -5403,19 +5427,19 @@
         <v>352.9</v>
       </c>
       <c r="AI41">
-        <v>0.038</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="AJ41">
         <v>0.8</v>
       </c>
       <c r="AK41">
-        <v>51.733</v>
+        <v>51.732999999999997</v>
       </c>
       <c r="AL41">
-        <v>0.011</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:38">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>400</v>
       </c>
@@ -5462,19 +5486,19 @@
         <v>128.4</v>
       </c>
       <c r="P42">
-        <v>0.06900000000000001</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="Q42">
-        <v>0.061</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="R42">
-        <v>0.058</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="S42">
-        <v>0.062</v>
+        <v>6.2E-2</v>
       </c>
       <c r="T42">
-        <v>0.089</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="U42">
         <v>3.3</v>
@@ -5507,10 +5531,10 @@
         <v>1.2</v>
       </c>
       <c r="AE42">
-        <v>65.09999999999999</v>
+        <v>65.099999999999994</v>
       </c>
       <c r="AF42">
-        <v>0.08500000000000001</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="AG42">
         <v>651</v>
@@ -5519,7 +5543,7 @@
         <v>952.3</v>
       </c>
       <c r="AI42">
-        <v>0.065</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="AJ42">
         <v>1.2</v>
@@ -5528,10 +5552,10 @@
         <v>121.48</v>
       </c>
       <c r="AL42">
-        <v>0.0125</v>
+        <v>1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:38">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>410</v>
       </c>
@@ -5572,22 +5596,22 @@
         <v>52.4</v>
       </c>
       <c r="N43">
-        <v>0.052</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="O43">
         <v>9.5</v>
       </c>
       <c r="P43">
-        <v>0.028</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="Q43">
-        <v>0.025</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="R43">
-        <v>0.068</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="S43">
-        <v>0.004</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="T43">
         <v>0.1</v>
@@ -5599,10 +5623,10 @@
         <v>0.1</v>
       </c>
       <c r="W43">
-        <v>0.07199999999999999</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="X43">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="Y43">
         <v>0.02</v>
@@ -5611,22 +5635,22 @@
         <v>1</v>
       </c>
       <c r="AA43">
-        <v>0.018</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="AB43">
         <v>3.1</v>
       </c>
       <c r="AC43">
-        <v>0.062</v>
+        <v>6.2E-2</v>
       </c>
       <c r="AD43">
-        <v>0.08500000000000001</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="AE43">
         <v>2.8</v>
       </c>
       <c r="AF43">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="AG43">
         <v>56.3</v>
@@ -5635,19 +5659,19 @@
         <v>30.9</v>
       </c>
       <c r="AI43">
-        <v>0.059</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="AJ43">
         <v>0.1</v>
       </c>
       <c r="AK43">
-        <v>9.553000000000001</v>
+        <v>9.5530000000000008</v>
       </c>
       <c r="AL43">
-        <v>0.028</v>
+        <v>2.8000000000000001E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:38">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>420</v>
       </c>
@@ -5670,7 +5694,7 @@
         <v>17.7</v>
       </c>
       <c r="H44">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I44">
         <v>0</v>
@@ -5703,7 +5727,7 @@
         <v>0.1</v>
       </c>
       <c r="S44">
-        <v>0.065</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="T44">
         <v>0.5</v>
@@ -5742,7 +5766,7 @@
         <v>375.8</v>
       </c>
       <c r="AF44">
-        <v>0.074</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="AG44">
         <v>1142.7</v>
@@ -5760,10 +5784,10 @@
         <v>222.5</v>
       </c>
       <c r="AL44">
-        <v>0.035</v>
+        <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:38">
+    <row r="45" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>430</v>
       </c>
@@ -5780,7 +5804,7 @@
         <v>3.2</v>
       </c>
       <c r="F45">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G45">
         <v>1.2</v>
@@ -5807,19 +5831,19 @@
         <v>0.2</v>
       </c>
       <c r="O45">
-        <v>286.4</v>
+        <v>286.39999999999998</v>
       </c>
       <c r="P45">
-        <v>0.032</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="Q45">
         <v>0.3</v>
       </c>
       <c r="R45">
-        <v>0.022</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="S45">
-        <v>0.021</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="T45">
         <v>0.2</v>
@@ -5846,7 +5870,7 @@
         <v>0</v>
       </c>
       <c r="AB45">
-        <v>35.2</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="AC45">
         <v>0.1</v>
@@ -5858,7 +5882,7 @@
         <v>45.8</v>
       </c>
       <c r="AF45">
-        <v>0.003</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="AG45">
         <v>704</v>
@@ -5873,13 +5897,13 @@
         <v>3.6</v>
       </c>
       <c r="AK45">
-        <v>98.078</v>
+        <v>98.078000000000003</v>
       </c>
       <c r="AL45">
-        <v>0.008</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:38">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>440</v>
       </c>
@@ -5920,22 +5944,22 @@
         <v>50</v>
       </c>
       <c r="N46">
-        <v>0.08599999999999999</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="O46">
-        <v>93.09999999999999</v>
+        <v>93.1</v>
       </c>
       <c r="P46">
-        <v>0.038</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="Q46">
-        <v>0.033</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="R46">
-        <v>0.038</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="S46">
-        <v>0.037</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="T46">
         <v>0.2</v>
@@ -5965,16 +5989,16 @@
         <v>12.2</v>
       </c>
       <c r="AC46">
-        <v>0.061</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="AD46">
         <v>1</v>
       </c>
       <c r="AE46">
-        <v>37.8</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="AF46">
-        <v>0.032</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="AG46">
         <v>248.9</v>
@@ -5989,13 +6013,13 @@
         <v>0.5</v>
       </c>
       <c r="AK46">
-        <v>37.228</v>
+        <v>37.228000000000002</v>
       </c>
       <c r="AL46">
-        <v>0.008999999999999999</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:38">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>450</v>
       </c>
@@ -6036,25 +6060,25 @@
         <v>14.7</v>
       </c>
       <c r="N47">
-        <v>0.098</v>
+        <v>9.8000000000000004E-2</v>
       </c>
       <c r="O47">
-        <v>20.1</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="P47">
-        <v>0.099</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="Q47">
-        <v>0.091</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="R47">
         <v>0.09</v>
       </c>
       <c r="S47">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="T47">
-        <v>0.027</v>
+        <v>2.7E-2</v>
       </c>
       <c r="U47">
         <v>1.8</v>
@@ -6081,37 +6105,37 @@
         <v>14.4</v>
       </c>
       <c r="AC47">
-        <v>0.021</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AD47">
-        <v>0.057</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="AE47">
         <v>8.5</v>
       </c>
       <c r="AF47">
-        <v>0.08799999999999999</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="AG47">
         <v>45.8</v>
       </c>
       <c r="AH47">
-        <v>82.59999999999999</v>
+        <v>82.6</v>
       </c>
       <c r="AI47">
-        <v>0.042</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="AJ47">
         <v>0.2</v>
       </c>
       <c r="AK47">
-        <v>22.203</v>
+        <v>22.202999999999999</v>
       </c>
       <c r="AL47">
-        <v>0.008500000000000001</v>
+        <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:38">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>460</v>
       </c>
@@ -6155,7 +6179,7 @@
         <v>0.2</v>
       </c>
       <c r="O48">
-        <v>274.1</v>
+        <v>274.10000000000002</v>
       </c>
       <c r="P48">
         <v>0.4</v>
@@ -6164,7 +6188,7 @@
         <v>0.4</v>
       </c>
       <c r="R48">
-        <v>0.094</v>
+        <v>9.4E-2</v>
       </c>
       <c r="S48">
         <v>0.1</v>
@@ -6197,16 +6221,16 @@
         <v>135.1</v>
       </c>
       <c r="AC48">
-        <v>0.037</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="AD48">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="AE48">
         <v>212.3</v>
       </c>
       <c r="AF48">
-        <v>0.077</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="AG48">
         <v>648.5</v>
@@ -6224,10 +6248,10 @@
         <v>251.3</v>
       </c>
       <c r="AL48">
-        <v>0.018</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:38">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>470</v>
       </c>
@@ -6265,7 +6289,7 @@
         <v>0</v>
       </c>
       <c r="M49">
-        <v>78.40000000000001</v>
+        <v>78.400000000000006</v>
       </c>
       <c r="N49">
         <v>0.1</v>
@@ -6274,22 +6298,22 @@
         <v>71.2</v>
       </c>
       <c r="P49">
-        <v>0.019</v>
+        <v>1.9E-2</v>
       </c>
       <c r="Q49">
         <v>0.2</v>
       </c>
       <c r="R49">
-        <v>0.007</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="S49">
-        <v>0.047</v>
+        <v>4.7E-2</v>
       </c>
       <c r="T49">
         <v>0.3</v>
       </c>
       <c r="U49">
-        <v>10.2</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="V49">
         <v>1</v>
@@ -6307,22 +6331,22 @@
         <v>1.7</v>
       </c>
       <c r="AA49">
-        <v>0.025</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AB49">
         <v>13.4</v>
       </c>
       <c r="AC49">
-        <v>0.027</v>
+        <v>2.7E-2</v>
       </c>
       <c r="AD49">
         <v>1.8</v>
       </c>
       <c r="AE49">
-        <v>85.09999999999999</v>
+        <v>85.1</v>
       </c>
       <c r="AF49">
-        <v>0.015</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="AG49">
         <v>243</v>
@@ -6331,19 +6355,19 @@
         <v>351.7</v>
       </c>
       <c r="AI49">
-        <v>0.067</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="AJ49">
         <v>0.7</v>
       </c>
       <c r="AK49">
-        <v>52.063</v>
+        <v>52.063000000000002</v>
       </c>
       <c r="AL49">
-        <v>0.0095</v>
+        <v>9.4999999999999998E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:38">
+    <row r="50" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>480</v>
       </c>
@@ -6381,13 +6405,13 @@
         <v>0</v>
       </c>
       <c r="M50">
-        <v>94.90000000000001</v>
+        <v>94.9</v>
       </c>
       <c r="N50">
         <v>0.1</v>
       </c>
       <c r="O50">
-        <v>148.2</v>
+        <v>148.19999999999999</v>
       </c>
       <c r="P50">
         <v>0.1</v>
@@ -6396,13 +6420,13 @@
         <v>0.2</v>
       </c>
       <c r="R50">
-        <v>0.023</v>
+        <v>2.3E-2</v>
       </c>
       <c r="S50">
-        <v>0.083</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="T50">
-        <v>0.035</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="U50">
         <v>0.8</v>
@@ -6429,37 +6453,37 @@
         <v>42.4</v>
       </c>
       <c r="AC50">
-        <v>0.063</v>
+        <v>6.3E-2</v>
       </c>
       <c r="AD50">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="AE50">
         <v>74.7</v>
       </c>
       <c r="AF50">
-        <v>0.075</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="AG50">
-        <v>288.9</v>
+        <v>288.89999999999998</v>
       </c>
       <c r="AH50">
         <v>959.5</v>
       </c>
       <c r="AI50">
-        <v>0.08799999999999999</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="AJ50">
         <v>1</v>
       </c>
       <c r="AK50">
-        <v>97.59999999999999</v>
+        <v>97.6</v>
       </c>
       <c r="AL50">
-        <v>0.015</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:38">
+    <row r="51" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>490</v>
       </c>
@@ -6491,7 +6515,7 @@
         <v>0</v>
       </c>
       <c r="K51">
-        <v>84.40000000000001</v>
+        <v>84.4</v>
       </c>
       <c r="L51">
         <v>0</v>
@@ -6512,19 +6536,19 @@
         <v>0.7</v>
       </c>
       <c r="R51">
-        <v>0.073</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="S51">
-        <v>0.065</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="T51">
         <v>0.5</v>
       </c>
       <c r="U51">
-        <v>32.2</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="V51">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="W51">
         <v>2.4</v>
@@ -6533,13 +6557,13 @@
         <v>0</v>
       </c>
       <c r="Y51">
-        <v>0.08599999999999999</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="Z51">
         <v>3.8</v>
       </c>
       <c r="AA51">
-        <v>0.021</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="AB51">
         <v>39.6</v>
@@ -6554,10 +6578,10 @@
         <v>118.8</v>
       </c>
       <c r="AF51">
-        <v>0.064</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="AG51">
-        <v>1053.4</v>
+        <v>1053.4000000000001</v>
       </c>
       <c r="AH51">
         <v>1358.3</v>
@@ -6575,7 +6599,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="52" spans="1:38">
+    <row r="52" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>500</v>
       </c>
@@ -6622,7 +6646,7 @@
         <v>235.9</v>
       </c>
       <c r="P52">
-        <v>0.046</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="Q52">
         <v>0.3</v>
@@ -6649,13 +6673,13 @@
         <v>3.1</v>
       </c>
       <c r="Y52">
-        <v>0.066</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="Z52">
         <v>2.6</v>
       </c>
       <c r="AA52">
-        <v>0.063</v>
+        <v>6.3E-2</v>
       </c>
       <c r="AB52">
         <v>65.5</v>
@@ -6670,7 +6694,7 @@
         <v>127.9</v>
       </c>
       <c r="AF52">
-        <v>0.061</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="AG52">
         <v>811.2</v>
@@ -6685,13 +6709,13 @@
         <v>1.8</v>
       </c>
       <c r="AK52">
-        <v>143.814</v>
+        <v>143.81399999999999</v>
       </c>
       <c r="AL52">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:38">
+    <row r="53" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>510</v>
       </c>
@@ -6738,19 +6762,19 @@
         <v>103.9</v>
       </c>
       <c r="P53">
-        <v>0.018</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="Q53">
-        <v>0.005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="R53">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="S53">
         <v>0.02</v>
       </c>
       <c r="T53">
-        <v>0.07000000000000001</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="U53">
         <v>1.8</v>
@@ -6762,7 +6786,7 @@
         <v>0.2</v>
       </c>
       <c r="X53">
-        <v>10.2</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="Y53">
         <v>0</v>
@@ -6774,7 +6798,7 @@
         <v>0</v>
       </c>
       <c r="AB53">
-        <v>79.09999999999999</v>
+        <v>79.099999999999994</v>
       </c>
       <c r="AC53">
         <v>1.6</v>
@@ -6783,10 +6807,10 @@
         <v>1</v>
       </c>
       <c r="AE53">
-        <v>84.40000000000001</v>
+        <v>84.4</v>
       </c>
       <c r="AF53">
-        <v>0.093</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="AG53">
         <v>375.2</v>
@@ -6795,19 +6819,19 @@
         <v>351.1</v>
       </c>
       <c r="AI53">
-        <v>0.003</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="AJ53">
-        <v>10.2</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="AK53">
         <v>118.35</v>
       </c>
       <c r="AL53">
-        <v>0.042</v>
+        <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:38">
+    <row r="54" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>520</v>
       </c>
@@ -6824,13 +6848,13 @@
         <v>0.3</v>
       </c>
       <c r="F54">
-        <v>0.002</v>
+        <v>2E-3</v>
       </c>
       <c r="G54">
-        <v>0.042</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="H54">
-        <v>0.038</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="I54">
         <v>0.6</v>
@@ -6848,25 +6872,25 @@
         <v>13.6</v>
       </c>
       <c r="N54">
-        <v>0.064</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="O54">
         <v>22.7</v>
       </c>
       <c r="P54">
-        <v>0.059</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="Q54">
-        <v>0.066</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="R54">
-        <v>0.008999999999999999</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="S54">
-        <v>0.043</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="T54">
-        <v>0.064</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="U54">
         <v>0.6</v>
@@ -6887,7 +6911,7 @@
         <v>0.3</v>
       </c>
       <c r="AA54">
-        <v>0.074</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="AB54">
         <v>15</v>
@@ -6902,16 +6926,16 @@
         <v>8.5</v>
       </c>
       <c r="AF54">
-        <v>0.019</v>
+        <v>1.9E-2</v>
       </c>
       <c r="AG54">
         <v>52.6</v>
       </c>
       <c r="AH54">
-        <v>99.09999999999999</v>
+        <v>99.1</v>
       </c>
       <c r="AI54">
-        <v>0.044</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="AJ54">
         <v>0.5</v>
@@ -6920,10 +6944,10 @@
         <v>23.044</v>
       </c>
       <c r="AL54">
-        <v>0.015</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:38">
+    <row r="55" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>530</v>
       </c>
@@ -6949,7 +6973,7 @@
         <v>0.3</v>
       </c>
       <c r="I55">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="J55">
         <v>0</v>
@@ -6961,25 +6985,25 @@
         <v>0</v>
       </c>
       <c r="M55">
-        <v>82.59999999999999</v>
+        <v>82.6</v>
       </c>
       <c r="N55">
         <v>0.2</v>
       </c>
       <c r="O55">
-        <v>88.09999999999999</v>
+        <v>88.1</v>
       </c>
       <c r="P55">
-        <v>0.099</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="Q55">
-        <v>0.06900000000000001</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="R55">
         <v>0.2</v>
       </c>
       <c r="S55">
-        <v>0.08799999999999999</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="T55">
         <v>0.1</v>
@@ -6991,7 +7015,7 @@
         <v>0</v>
       </c>
       <c r="W55">
-        <v>0.095</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="X55">
         <v>0</v>
@@ -7003,7 +7027,7 @@
         <v>8</v>
       </c>
       <c r="AA55">
-        <v>0.016</v>
+        <v>1.6E-2</v>
       </c>
       <c r="AB55">
         <v>124.5</v>
@@ -7021,25 +7045,25 @@
         <v>0</v>
       </c>
       <c r="AG55">
-        <v>275.6</v>
+        <v>275.60000000000002</v>
       </c>
       <c r="AH55">
         <v>207</v>
       </c>
       <c r="AI55">
-        <v>0.007</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="AJ55">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="AK55">
         <v>163.446</v>
       </c>
       <c r="AL55">
-        <v>0.013</v>
+        <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:38">
+    <row r="56" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>540</v>
       </c>
@@ -7080,7 +7104,7 @@
         <v>10.4</v>
       </c>
       <c r="N56">
-        <v>0.015</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="O56">
         <v>9.4</v>
@@ -7089,25 +7113,25 @@
         <v>0</v>
       </c>
       <c r="Q56">
-        <v>0.026</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="R56">
-        <v>0.003</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="S56">
-        <v>0.016</v>
+        <v>1.6E-2</v>
       </c>
       <c r="T56">
-        <v>0.08400000000000001</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="U56">
         <v>0.2</v>
       </c>
       <c r="V56">
-        <v>0.081</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="W56">
-        <v>0.007</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="X56">
         <v>0.6</v>
@@ -7134,7 +7158,7 @@
         <v>8.5</v>
       </c>
       <c r="AF56">
-        <v>0.063</v>
+        <v>6.3E-2</v>
       </c>
       <c r="AG56">
         <v>23.2</v>
@@ -7143,7 +7167,7 @@
         <v>35.6</v>
       </c>
       <c r="AI56">
-        <v>0.092</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="AJ56">
         <v>12.7</v>
@@ -7152,10 +7176,10 @@
         <v>15.5</v>
       </c>
       <c r="AL56">
-        <v>0.025</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:38">
+    <row r="57" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>550</v>
       </c>
@@ -7196,22 +7220,22 @@
         <v>167.4</v>
       </c>
       <c r="N57">
-        <v>0.065</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="O57">
         <v>25.8</v>
       </c>
       <c r="P57">
-        <v>0.047</v>
+        <v>4.7E-2</v>
       </c>
       <c r="Q57">
         <v>0.5</v>
       </c>
       <c r="R57">
-        <v>0.078</v>
+        <v>7.8E-2</v>
       </c>
       <c r="S57">
-        <v>0.08799999999999999</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="T57">
         <v>0.6</v>
@@ -7244,13 +7268,13 @@
         <v>0.2</v>
       </c>
       <c r="AD57">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="AE57">
         <v>62.6</v>
       </c>
       <c r="AF57">
-        <v>0.048</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="AG57">
         <v>702</v>
@@ -7259,16 +7283,16 @@
         <v>1036.8</v>
       </c>
       <c r="AI57">
-        <v>0.026</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="AJ57">
         <v>1.2</v>
       </c>
       <c r="AK57">
-        <v>141.587</v>
+        <v>141.58699999999999</v>
       </c>
       <c r="AL57">
-        <v>0.038</v>
+        <v>3.7999999999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>